<commit_message>
Actualizacion y cierre de no conformidades
</commit_message>
<xml_diff>
--- a/Proyectos/2015/11/P1319 - CCON,CNOM, Jeniffer Venegas _MO/Calidad/No_conformidades.xlsx
+++ b/Proyectos/2015/11/P1319 - CCON,CNOM, Jeniffer Venegas _MO/Calidad/No_conformidades.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>REPORTE DE NO CONFORMIDADES</t>
   </si>
@@ -47,7 +47,10 @@
     <t>Oriana Osiris</t>
   </si>
   <si>
-    <t>En proceso</t>
+    <t>Cerrada</t>
+  </si>
+  <si>
+    <t>Se omite debido a que no se requiere la etapa de cambios para el proyecto</t>
   </si>
   <si>
     <t>Falta agregar la complejidad en tiempo de implementación</t>
@@ -56,10 +59,10 @@
     <t>No se cuenta con evidencia de envío de carta de aceptación al cliente</t>
   </si>
   <si>
-    <t>Notificación de no conformidades</t>
-  </si>
-  <si>
-    <t>Cerrada</t>
+    <t>Se muestra evidencia en Deal del cliente</t>
+  </si>
+  <si>
+    <t>Notificación de creación lineas base</t>
   </si>
   <si>
     <t>Es importante notificar por correo el momento de la creación de la Línea base así como el registro de dicha tarea</t>
@@ -321,8 +324,8 @@
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -381,7 +384,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
         <v>1</v>
       </c>
@@ -394,18 +397,22 @@
       <c r="D4" s="5" t="n">
         <v>42331</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="5" t="n">
+        <v>42331</v>
+      </c>
       <c r="F4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="4"/>
+      <c r="G4" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>9</v>
@@ -413,7 +420,9 @@
       <c r="D5" s="5" t="n">
         <v>42331</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="5" t="n">
+        <v>42331</v>
+      </c>
       <c r="F5" s="6" t="s">
         <v>10</v>
       </c>
@@ -424,7 +433,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>9</v>
@@ -432,18 +441,22 @@
       <c r="D6" s="5" t="n">
         <v>42333</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="5" t="n">
+        <v>42331</v>
+      </c>
       <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
         <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>9</v>
@@ -455,10 +468,10 @@
         <v>42331</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -466,7 +479,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>9</v>
@@ -474,7 +487,9 @@
       <c r="D8" s="5" t="n">
         <v>42331</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="5" t="n">
+        <v>42331</v>
+      </c>
       <c r="F8" s="6" t="s">
         <v>10</v>
       </c>
@@ -485,7 +500,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>9</v>
@@ -497,10 +512,10 @@
         <v>42331</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -508,7 +523,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>9</v>
@@ -520,10 +535,10 @@
         <v>42331</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>